<commit_message>
SVGs for the master thesis
</commit_message>
<xml_diff>
--- a/Time-test/Time-test.xlsx
+++ b/Time-test/Time-test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hallv\Prosjekt\Skole\Master-s-Thesis-AutoTrust\Time-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824DAF11-1433-476B-B4E5-C0A6EECBD18C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A984D0E7-E603-4E70-9942-2D055769FBC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AB1CF54C-FF1B-4144-91C1-3949042FA010}"/>
   </bookViews>
@@ -128,7 +128,7 @@
     <t>Average</t>
   </si>
   <si>
-    <t>All the time is in seconds!</t>
+    <t>Note: The time is in seconds</t>
   </si>
 </sst>
 </file>
@@ -677,10 +677,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K14"/>
+  <dimension ref="A3:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,13 +698,6 @@
     <col min="11" max="11" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-    </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>0</v>
@@ -1132,9 +1125,16 @@
         <v>1.7866</v>
       </c>
     </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A15:C15"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="61" orientation="landscape" r:id="rId1"/>

</xml_diff>